<commit_message>
adding presentation images for README
</commit_message>
<xml_diff>
--- a/presentation/model_performance.xlsx
+++ b/presentation/model_performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbywilkinson/HackTheMachine/start-here/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbywilkinson/Library/Mobile Documents/com~apple~CloudDocs/HackTheMachine/presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC47CA9-7F36-6B45-A118-6C635EF4F73E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847F485B-4D2C-244C-8DCD-F7205E9AFDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" xr2:uid="{6A2C629D-9BF7-194D-B7CA-3471731CD277}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="27820" windowHeight="17040" xr2:uid="{6A2C629D-9BF7-194D-B7CA-3471731CD277}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>F1</t>
   </si>
   <si>
-    <t>Random Forst</t>
+    <t>Random Forest</t>
   </si>
 </sst>
 </file>
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,13 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -429,97 +438,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AD5EB0-741C-994B-8368-1E732853C59B}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.55200000000000005</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.37</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.72099999999999997</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.72</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.73</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.52</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.745</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.72</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.8</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.76</v>
       </c>
     </row>

</xml_diff>